<commit_message>
Added solution for 450 worksheet
</commit_message>
<xml_diff>
--- a/WorkSheets/450_by_love_babbar.xlsx
+++ b/WorkSheets/450_by_love_babbar.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1420,6 +1420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1851,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1894,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">

</xml_diff>